<commit_message>
fixed file path issue where it only worked on my system
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
+++ b/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="192">
   <si>
     <t>Subject Code</t>
   </si>
@@ -596,6 +596,15 @@
   </si>
   <si>
     <t>FACTORIO204</t>
+  </si>
+  <si>
+    <t>ENG1210</t>
+  </si>
+  <si>
+    <t>Intro to Coding</t>
+  </si>
+  <si>
+    <t>fortnite</t>
   </si>
 </sst>
 </file>
@@ -901,7 +910,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -909,7 +918,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.203125"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.90234375"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="14.06640625"/>
     <col min="3" max="26" customWidth="true" width="18.0"/>
   </cols>
@@ -980,10 +989,18 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>187</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>180</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Faculty, student, admin support. v1, still has some problems working on them
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
+++ b/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="193">
   <si>
     <t>Subject Code</t>
   </si>
@@ -965,18 +965,18 @@
     </row>
     <row r="4" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>184</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>184</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed all the problems for role based control
ALI THIS VERSION WORKS FOR EVERYTHING FOR PRESENTING
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
+++ b/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="203">
   <si>
     <t>Subject Code</t>
   </si>
@@ -609,6 +609,36 @@
   </si>
   <si>
     <t>Ali</t>
+  </si>
+  <si>
+    <t>TEst1</t>
+  </si>
+  <si>
+    <t>TESTY</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>TEST2</t>
+  </si>
+  <si>
+    <t>foty</t>
+  </si>
+  <si>
+    <t>ert</t>
+  </si>
+  <si>
+    <t>qwe</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>67jj</t>
+  </si>
+  <si>
+    <t>bnvbnvn</t>
   </si>
 </sst>
 </file>
@@ -926,7 +956,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -934,8 +964,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.88671875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.109375"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.2265625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.06640625"/>
     <col min="3" max="26" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
@@ -965,58 +995,42 @@
     </row>
     <row r="4" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>184</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>184</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>184</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
+    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
-        <v>181</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
-        <v>180</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>183</v>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added working and interactable calander to the event interface. Just needs to take tasks now
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
+++ b/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliMe\IdeaProjects\Version244pm\src\main\java\com\example\universitymanagementsystem\ExcelDatabase\"/>
     </mc:Choice>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="185">
   <si>
     <t>Subject Code</t>
   </si>
@@ -569,12 +569,28 @@
   </si>
   <si>
     <t>qwe</t>
+  </si>
+  <si>
+    <t>ENG1420</t>
+  </si>
+  <si>
+    <t>OPP Programming</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>OPP</t>
+  </si>
+  <si>
+    <t>ENG1440</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,9 +905,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="18" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.2265625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.00390625"/>
+    <col min="3" max="26" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -943,18 +959,18 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>179</v>
       </c>
     </row>
@@ -974,17 +990,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="27" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="7" customWidth="1"/>
-    <col min="10" max="26" width="10.85546875" style="7" customWidth="1"/>
-    <col min="27" max="16384" width="12.5703125" style="7"/>
+    <col min="1" max="1" customWidth="true" style="17" width="12.28515625"/>
+    <col min="2" max="2" customWidth="true" style="7" width="27.0"/>
+    <col min="3" max="3" customWidth="true" style="7" width="12.7109375"/>
+    <col min="4" max="4" customWidth="true" style="7" width="15.42578125"/>
+    <col min="5" max="5" customWidth="true" style="17" width="8.7109375"/>
+    <col min="6" max="6" customWidth="true" style="7" width="16.85546875"/>
+    <col min="7" max="7" customWidth="true" style="21" width="20.5703125"/>
+    <col min="8" max="8" customWidth="true" style="7" width="9.5703125"/>
+    <col min="9" max="9" customWidth="true" style="7" width="16.5703125"/>
+    <col min="10" max="26" customWidth="true" style="7" width="10.85546875"/>
+    <col min="27" max="16384" style="7" width="12.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2311,12 +2327,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" style="7"/>
-    <col min="5" max="5" width="33.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="7"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="10.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="7" width="12.42578125"/>
+    <col min="3" max="4" style="7" width="8.85546875"/>
+    <col min="5" max="5" customWidth="true" style="7" width="33.28515625"/>
+    <col min="6" max="6" customWidth="true" style="7" width="21.5703125"/>
+    <col min="7" max="16384" style="7" width="8.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2755,15 +2771,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="26" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.5703125"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="8.42578125"/>
+    <col min="4" max="4" customWidth="true" width="22.42578125"/>
+    <col min="5" max="5" customWidth="true" width="21.7109375"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625"/>
+    <col min="7" max="7" customWidth="true" width="20.0"/>
+    <col min="8" max="8" customWidth="true" width="9.42578125"/>
+    <col min="9" max="26" customWidth="true" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3916,16 +3932,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="52.28515625" customWidth="1"/>
-    <col min="10" max="26" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.42578125"/>
+    <col min="2" max="2" customWidth="true" width="18.85546875"/>
+    <col min="3" max="3" customWidth="true" width="18.5703125"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125"/>
+    <col min="6" max="6" customWidth="true" width="8.5703125"/>
+    <col min="7" max="7" customWidth="true" width="9.85546875"/>
+    <col min="8" max="8" customWidth="true" width="13.28515625"/>
+    <col min="9" max="9" customWidth="true" width="52.28515625"/>
+    <col min="10" max="26" customWidth="true" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
I fixed the different size windows issue and now everything is fullscreen. I created a class to unify interface movement which helps clean up the code a lot
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
+++ b/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliMe\IdeaProjects\Version244pm\src\main\java\com\example\universitymanagementsystem\ExcelDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5418DAC0-43B7-4DC3-8997-487621EFCB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B090D360-EAE2-494C-9126-724C5AACD863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="3750" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="181">
   <si>
     <t>Subject Code</t>
   </si>
@@ -412,9 +412,6 @@
     <t>S20250010</t>
   </si>
   <si>
-    <t>Jennifer Davis</t>
-  </si>
-  <si>
     <t>555 Oakwood Pl.</t>
   </si>
   <si>
@@ -571,19 +568,10 @@
     <t>qwe</t>
   </si>
   <si>
-    <t>ENG1420</t>
-  </si>
-  <si>
-    <t>OPP Programming</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>OPP</t>
-  </si>
-  <si>
-    <t>ENG1440</t>
+    <t>Jennifer Russel</t>
+  </si>
+  <si>
+    <t>555-3457</t>
   </si>
 </sst>
 </file>
@@ -905,8 +893,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.2265625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.00390625"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.0"/>
     <col min="3" max="26" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
@@ -960,18 +948,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s" s="0">
+        <v>175</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>176</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s" s="0">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -2321,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D458A2-78A0-4890-A85A-AD55AFB8F75E}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,7 +2378,7 @@
         <v>69</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>70</v>
@@ -2504,7 +2492,7 @@
         <v>92</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>70</v>
@@ -2536,13 +2524,13 @@
         <v>96</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>98</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>70</v>
@@ -2618,7 +2606,7 @@
         <v>111</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>70</v>
@@ -2694,7 +2682,7 @@
         <v>124</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>70</v>
@@ -2720,16 +2708,16 @@
         <v>126</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>79</v>
@@ -2744,7 +2732,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K11" s="6">
         <v>0.2</v>
@@ -2784,25 +2772,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>64</v>
@@ -2810,19 +2798,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>39</v>
@@ -2836,19 +2824,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>46</v>
@@ -2862,25 +2850,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>73</v>
@@ -2888,19 +2876,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>39</v>
@@ -2914,22 +2902,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>49</v>
@@ -3946,45 +3934,45 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="E2" s="3">
         <v>45901.416666666664</v>
@@ -3993,27 +3981,27 @@
         <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="E3" s="3">
         <v>45935.583333333336</v>
@@ -4022,13 +4010,13 @@
         <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>71</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Worked on student profile image
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
+++ b/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliMe\IdeaProjects\Version244pm\src\main\java\com\example\universitymanagementsystem\ExcelDatabase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khale\IdeaProjects\NewUniversityManagementSystem\src\main\java\com\example\universitymanagementsystem\ExcelDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A41E727-8D8E-4BB0-811D-44BBD70FAC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8C92FE-C859-43B0-B3C0-2EF0EE2BF834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12192" yWindow="0" windowWidth="12480" windowHeight="14736" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="187">
   <si>
     <t>Subject Code</t>
   </si>
@@ -569,12 +569,34 @@
   </si>
   <si>
     <t>555-3457</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>default.png</t>
+  </si>
+  <si>
+    <t>file:/C:/Users/khale/IdeaProjects/NewUniversityManagementSystem/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/studentprofileimages/2.png</t>
+  </si>
+  <si>
+    <t>2.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -888,9 +910,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="18" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.33203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.0"/>
+    <col min="3" max="26" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -942,18 +964,18 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>177</v>
       </c>
     </row>
@@ -973,17 +995,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="27" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="20" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" style="6" customWidth="1"/>
-    <col min="10" max="26" width="10.88671875" style="6" customWidth="1"/>
-    <col min="27" max="16384" width="12.5546875" style="6"/>
+    <col min="1" max="1" customWidth="true" style="16" width="12.33203125"/>
+    <col min="2" max="2" customWidth="true" style="6" width="27.0"/>
+    <col min="3" max="3" customWidth="true" style="6" width="12.6640625"/>
+    <col min="4" max="4" customWidth="true" style="6" width="15.44140625"/>
+    <col min="5" max="5" customWidth="true" style="16" width="8.6640625"/>
+    <col min="6" max="6" customWidth="true" style="6" width="16.88671875"/>
+    <col min="7" max="7" customWidth="true" style="20" width="20.5546875"/>
+    <col min="8" max="8" customWidth="true" style="6" width="9.5546875"/>
+    <col min="9" max="9" customWidth="true" style="6" width="16.5546875"/>
+    <col min="10" max="26" customWidth="true" style="6" width="10.88671875"/>
+    <col min="27" max="16384" style="6" width="12.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2304,18 +2326,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D458A2-78A0-4890-A85A-AD55AFB8F75E}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="6"/>
-    <col min="5" max="5" width="33.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="10.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="12.44140625"/>
+    <col min="3" max="4" style="6" width="8.88671875"/>
+    <col min="5" max="5" customWidth="true" style="6" width="33.33203125"/>
+    <col min="6" max="6" customWidth="true" style="6" width="21.5546875"/>
+    <col min="7" max="16384" style="6" width="8.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -2379,7 +2401,7 @@
         <v>70</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>3</v>
@@ -2387,8 +2409,8 @@
       <c r="J2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="8">
-        <v>0.4</v>
+      <c r="K2" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>73</v>
@@ -2417,7 +2439,7 @@
         <v>70</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>71</v>
+        <v>186</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>5</v>
@@ -2425,8 +2447,8 @@
       <c r="J3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="8">
-        <v>0.5</v>
+      <c r="K3" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>73</v>
@@ -2455,7 +2477,7 @@
         <v>70</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>86</v>
@@ -2463,8 +2485,8 @@
       <c r="J4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="8">
-        <v>0.5</v>
+      <c r="K4" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>73</v>
@@ -2493,7 +2515,7 @@
         <v>70</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>93</v>
@@ -2501,8 +2523,8 @@
       <c r="J5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="K5" s="8">
-        <v>0.6</v>
+      <c r="K5" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>73</v>
@@ -2531,7 +2553,7 @@
         <v>70</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>10</v>
@@ -2539,8 +2561,8 @@
       <c r="J6" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K6" s="5">
-        <v>0.5</v>
+      <c r="K6" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>73</v>
@@ -2569,7 +2591,7 @@
         <v>70</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>104</v>
@@ -2577,8 +2599,8 @@
       <c r="J7" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="5">
-        <v>0.5</v>
+      <c r="K7" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>73</v>
@@ -2607,7 +2629,7 @@
         <v>70</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>111</v>
@@ -2615,8 +2637,8 @@
       <c r="J8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K8" s="5">
-        <v>0.4</v>
+      <c r="K8" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>73</v>
@@ -2645,7 +2667,7 @@
         <v>70</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>71</v>
+        <v>185</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>117</v>
@@ -2653,8 +2675,8 @@
       <c r="J9" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="K9" s="5">
-        <v>0.5</v>
+      <c r="K9" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>73</v>
@@ -2683,7 +2705,7 @@
         <v>70</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>124</v>
@@ -2691,8 +2713,8 @@
       <c r="J10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K10" s="5">
-        <v>0.5</v>
+      <c r="K10" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>73</v>
@@ -2721,7 +2743,7 @@
         <v>70</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>10</v>
@@ -2729,8 +2751,8 @@
       <c r="J11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="K11" s="5">
-        <v>0.2</v>
+      <c r="K11" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>73</v>
@@ -2741,6 +2763,9 @@
     <hyperlink ref="E5" r:id="rId1" xr:uid="{21B754AA-1EDB-478B-87CF-7155F35DF322}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="K2:K11" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2754,15 +2779,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="26" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.5546875"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="8.44140625"/>
+    <col min="4" max="4" customWidth="true" width="22.44140625"/>
+    <col min="5" max="5" customWidth="true" width="21.6640625"/>
+    <col min="6" max="6" customWidth="true" width="14.33203125"/>
+    <col min="7" max="7" customWidth="true" width="20.0"/>
+    <col min="8" max="8" customWidth="true" width="9.44140625"/>
+    <col min="9" max="26" customWidth="true" width="8.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -3911,23 +3936,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="52.33203125" style="6" customWidth="1"/>
-    <col min="10" max="26" width="8.5546875" style="6" customWidth="1"/>
-    <col min="27" max="16384" width="12.5546875" style="6"/>
+    <col min="1" max="1" customWidth="true" style="6" width="10.44140625"/>
+    <col min="2" max="2" customWidth="true" style="6" width="18.88671875"/>
+    <col min="3" max="3" customWidth="true" style="6" width="18.5546875"/>
+    <col min="4" max="4" customWidth="true" style="6" width="10.88671875"/>
+    <col min="5" max="5" customWidth="true" style="6" width="14.5546875"/>
+    <col min="6" max="6" customWidth="true" style="6" width="8.5546875"/>
+    <col min="7" max="7" customWidth="true" style="6" width="9.88671875"/>
+    <col min="8" max="8" customWidth="true" style="6" width="13.33203125"/>
+    <col min="9" max="9" customWidth="true" style="6" width="52.33203125"/>
+    <col min="10" max="26" customWidth="true" style="6" width="8.5546875"/>
+    <col min="27" max="16384" style="6" width="12.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
working add, edit and deleting for coursemanagement from excel
</commit_message>
<xml_diff>
--- a/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
+++ b/src/main/java/com/example/universitymanagementsystem/ExcelDatabase/UMS_Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliMe\IdeaProjects\Version244pm\src\main\java\com\example\universitymanagementsystem\ExcelDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3097084-EA6D-4A82-9DFD-4C6C87FDF982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E024E81-8BF0-4FFC-AEC7-6FE5B1115EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="18432" windowHeight="10728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3012" yWindow="2436" windowWidth="18432" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subjects" sheetId="1" r:id="rId1"/>
-    <sheet name="Courses" sheetId="2" r:id="rId2"/>
+    <sheet name="Courses" sheetId="7" r:id="rId2"/>
     <sheet name="Student" sheetId="6" r:id="rId3"/>
     <sheet name="Faculties" sheetId="4" r:id="rId4"/>
     <sheet name="Events" sheetId="5" r:id="rId5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="198">
   <si>
     <t>Subject Code</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Computer Science</t>
   </si>
   <si>
-    <t>CHEM200</t>
-  </si>
-  <si>
     <t>ENGG402</t>
   </si>
   <si>
@@ -124,490 +121,508 @@
     <t>Prof. Emily Brontë</t>
   </si>
   <si>
+    <t>Room 201</t>
+  </si>
+  <si>
+    <t>Introduction to French</t>
+  </si>
+  <si>
+    <t>Room 202</t>
+  </si>
+  <si>
+    <t>Dr. Lakyn Copeland</t>
+  </si>
+  <si>
+    <t>Water Resources</t>
+  </si>
+  <si>
+    <t>Mon/Fri 9:00 - 10:30</t>
+  </si>
+  <si>
+    <t>Room 203</t>
+  </si>
+  <si>
+    <t>Dr. Albozr Gharabaghi</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Academic Level</t>
+  </si>
+  <si>
+    <t>Current Semester</t>
+  </si>
+  <si>
+    <t>Profile Photo</t>
+  </si>
+  <si>
+    <t>Subjects Registered</t>
+  </si>
+  <si>
+    <t>Thesis Title</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>S20250001</t>
+  </si>
+  <si>
+    <t>Alice Smith</t>
+  </si>
+  <si>
+    <t>123 Maple St.</t>
+  </si>
+  <si>
+    <t>555-1234</t>
+  </si>
+  <si>
+    <t>alice@example.edu</t>
+  </si>
+  <si>
+    <t>Fall 2025</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>default123</t>
+  </si>
+  <si>
+    <t>S20250002</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>456 Oak St.</t>
+  </si>
+  <si>
+    <t>555-5678</t>
+  </si>
+  <si>
+    <t>bob@example.edu</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
+  </si>
+  <si>
+    <t>S20250003</t>
+  </si>
+  <si>
+    <t>Carol Williams</t>
+  </si>
+  <si>
+    <t>789 Pine St.</t>
+  </si>
+  <si>
+    <t>555-9012</t>
+  </si>
+  <si>
+    <t>carol@example.edu</t>
+  </si>
+  <si>
+    <t>ENGG402, HIST101</t>
+  </si>
+  <si>
+    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
+  </si>
+  <si>
+    <t>S20250004</t>
+  </si>
+  <si>
+    <t>Lucka Racki</t>
+  </si>
+  <si>
+    <t>1767 Jane St.</t>
+  </si>
+  <si>
+    <t>439-9966</t>
+  </si>
+  <si>
+    <t>lucka@example.edu</t>
+  </si>
+  <si>
+    <t>Bio300</t>
+  </si>
+  <si>
+    <t>S20250005</t>
+  </si>
+  <si>
+    <t>David Lee</t>
+  </si>
+  <si>
+    <t>90 Elm St.</t>
+  </si>
+  <si>
+    <t>lee@example.edu</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>S20250006</t>
+  </si>
+  <si>
+    <t>Emily Brown</t>
+  </si>
+  <si>
+    <t>111 Oak Ave.</t>
+  </si>
+  <si>
+    <t>555-7890</t>
+  </si>
+  <si>
+    <t>brown@example.edu</t>
+  </si>
+  <si>
+    <t>Chem200</t>
+  </si>
+  <si>
+    <t>Synthesis and Characterization of Novel Catalysts</t>
+  </si>
+  <si>
+    <t>S20250007</t>
+  </si>
+  <si>
+    <t>George Smith</t>
+  </si>
+  <si>
+    <t>222 Pine Rd.</t>
+  </si>
+  <si>
+    <t>555-2345</t>
+  </si>
+  <si>
+    <t>smith@example.edu</t>
+  </si>
+  <si>
+    <t>Music102</t>
+  </si>
+  <si>
+    <t>S20250008</t>
+  </si>
+  <si>
+    <t>Helen Jones</t>
+  </si>
+  <si>
+    <t>333 Maple Dr.</t>
+  </si>
+  <si>
+    <t>555-4567</t>
+  </si>
+  <si>
+    <t>jones@example.edu</t>
+  </si>
+  <si>
+    <t>PSYCHO100, Music102, HIST101</t>
+  </si>
+  <si>
+    <t>The Effects of Stress on Cognitive Function</t>
+  </si>
+  <si>
+    <t>S20250009</t>
+  </si>
+  <si>
+    <t>Isaac Clark</t>
+  </si>
+  <si>
+    <t>444 Cedar Ln.</t>
+  </si>
+  <si>
+    <t>555-8901</t>
+  </si>
+  <si>
+    <t>clark@example.edu</t>
+  </si>
+  <si>
+    <t>BIo300</t>
+  </si>
+  <si>
+    <t>S20250010</t>
+  </si>
+  <si>
+    <t>555 Oakwood Pl.</t>
+  </si>
+  <si>
+    <t>davis@example.edu</t>
+  </si>
+  <si>
+    <t>The Renaissance: Art, Culture, and Society</t>
+  </si>
+  <si>
+    <t>Faculty ID</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Research Interest</t>
+  </si>
+  <si>
+    <t>Office Location</t>
+  </si>
+  <si>
+    <t>Courses Offered</t>
+  </si>
+  <si>
+    <t>F0001</t>
+  </si>
+  <si>
+    <t>Ph.D.</t>
+  </si>
+  <si>
+    <t>Computational Theory</t>
+  </si>
+  <si>
+    <t>turing@university.edu</t>
+  </si>
+  <si>
+    <t>F0002</t>
+  </si>
+  <si>
+    <t>Master's</t>
+  </si>
+  <si>
+    <t>English Literature</t>
+  </si>
+  <si>
+    <t>bronte@university.edu</t>
+  </si>
+  <si>
+    <t>F0003</t>
+  </si>
+  <si>
+    <t>Dr. Grace Hopper</t>
+  </si>
+  <si>
+    <t>Computer Programming</t>
+  </si>
+  <si>
+    <t>hopper@university.edu</t>
+  </si>
+  <si>
+    <t>Lab 203</t>
+  </si>
+  <si>
+    <t>Intro to Programming</t>
+  </si>
+  <si>
+    <t>F0004</t>
+  </si>
+  <si>
+    <t>copeland@university.edu</t>
+  </si>
+  <si>
+    <t>F0005</t>
+  </si>
+  <si>
+    <t>Albozr Gharabaghi</t>
+  </si>
+  <si>
+    <t>Water and Soil</t>
+  </si>
+  <si>
+    <t>gharabaghi@university.edu</t>
+  </si>
+  <si>
+    <t>Lab 202</t>
+  </si>
+  <si>
+    <t>Event Code</t>
+  </si>
+  <si>
+    <t>Event Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date and Time</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Header Image</t>
+  </si>
+  <si>
+    <t>Registered Students</t>
+  </si>
+  <si>
+    <t>EV001</t>
+  </si>
+  <si>
+    <t>Welcome Seminar</t>
+  </si>
+  <si>
+    <t>Orientation week</t>
+  </si>
+  <si>
+    <t>Auditorium</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Alice Smith, Bob Johnson,Jennifer Davis,Helen Jones</t>
+  </si>
+  <si>
+    <t>EV002</t>
+  </si>
+  <si>
+    <t>Research Workshop</t>
+  </si>
+  <si>
+    <t>Graduate workshop</t>
+  </si>
+  <si>
+    <t>Lab 301</t>
+  </si>
+  <si>
+    <t>Paid ($20)</t>
+  </si>
+  <si>
+    <t>Alice Smith, Bob Johnson, Lucka Racki,Helen Jones,David Lee</t>
+  </si>
+  <si>
+    <t>ENG1210</t>
+  </si>
+  <si>
+    <t>Intro to Coding</t>
+  </si>
+  <si>
+    <t>undergraduate</t>
+  </si>
+  <si>
+    <t>qwe</t>
+  </si>
+  <si>
+    <t>Jennifer Russel</t>
+  </si>
+  <si>
+    <t>555-3457</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>default.png</t>
+  </si>
+  <si>
+    <t>2.png</t>
+  </si>
+  <si>
+    <t>OnePiece.jpg</t>
+  </si>
+  <si>
+    <t>default1234</t>
+  </si>
+  <si>
+    <t>F0006</t>
+  </si>
+  <si>
+    <t>penis</t>
+  </si>
+  <si>
+    <t>balls</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>doeakdasd</t>
+  </si>
+  <si>
     <t>Section 2</t>
   </si>
   <si>
-    <t>Mon/Wed 10-12 PM</t>
-  </si>
-  <si>
-    <t>Introduction to Programming</t>
-  </si>
-  <si>
-    <t>Tue/Thu 12-2 PM</t>
-  </si>
-  <si>
-    <t>Room 103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prof. Bahar Nozari </t>
-  </si>
-  <si>
-    <t>Introduction to Chemistry</t>
-  </si>
-  <si>
-    <t>Mon/ Thu 3-4 PM</t>
-  </si>
-  <si>
-    <t>Room 201</t>
-  </si>
-  <si>
-    <t>Dr. Lucka Lucku</t>
-  </si>
-  <si>
-    <t>Mon/ Tue 5-6 PM</t>
-  </si>
-  <si>
-    <t>Section 3</t>
-  </si>
-  <si>
-    <t>Fri/ Thu 2-3 PM</t>
-  </si>
-  <si>
-    <t>Introduction to French</t>
-  </si>
-  <si>
-    <t>Tue/Thur 4:30 - 5:30 PM</t>
-  </si>
-  <si>
-    <t>Room 202</t>
-  </si>
-  <si>
-    <t>Dr. Lakyn Copeland</t>
-  </si>
-  <si>
-    <t>Tue/Thur 5:30 - 6:30 PM</t>
-  </si>
-  <si>
-    <t>Water Resources</t>
-  </si>
-  <si>
-    <t>Mon/Fri 9:00 - 10:30</t>
-  </si>
-  <si>
-    <t>Room 203</t>
-  </si>
-  <si>
-    <t>Dr. Albozr Gharabaghi</t>
-  </si>
-  <si>
-    <t>Student ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Telephone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Academic Level</t>
-  </si>
-  <si>
-    <t>Current Semester</t>
-  </si>
-  <si>
-    <t>Profile Photo</t>
-  </si>
-  <si>
-    <t>Subjects Registered</t>
-  </si>
-  <si>
-    <t>Thesis Title</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>S20250001</t>
-  </si>
-  <si>
-    <t>Alice Smith</t>
-  </si>
-  <si>
-    <t>123 Maple St.</t>
-  </si>
-  <si>
-    <t>555-1234</t>
-  </si>
-  <si>
-    <t>alice@example.edu</t>
-  </si>
-  <si>
-    <t>Fall 2025</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>default123</t>
-  </si>
-  <si>
-    <t>S20250002</t>
-  </si>
-  <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
-    <t>456 Oak St.</t>
-  </si>
-  <si>
-    <t>555-5678</t>
-  </si>
-  <si>
-    <t>bob@example.edu</t>
-  </si>
-  <si>
-    <t>Graduate</t>
-  </si>
-  <si>
-    <t>"The detection of oil under ice by remote mode conversion of ultrasound"</t>
-  </si>
-  <si>
-    <t>S20250003</t>
-  </si>
-  <si>
-    <t>Carol Williams</t>
-  </si>
-  <si>
-    <t>789 Pine St.</t>
-  </si>
-  <si>
-    <t>555-9012</t>
-  </si>
-  <si>
-    <t>carol@example.edu</t>
-  </si>
-  <si>
-    <t>ENGG402, HIST101</t>
-  </si>
-  <si>
-    <t>"On the economic optimality of marine reserves when fishing damages habitat"</t>
-  </si>
-  <si>
-    <t>S20250004</t>
-  </si>
-  <si>
-    <t>Lucka Racki</t>
-  </si>
-  <si>
-    <t>1767 Jane St.</t>
-  </si>
-  <si>
-    <t>439-9966</t>
-  </si>
-  <si>
-    <t>lucka@example.edu</t>
-  </si>
-  <si>
-    <t>Bio300</t>
-  </si>
-  <si>
-    <t>S20250005</t>
-  </si>
-  <si>
-    <t>David Lee</t>
-  </si>
-  <si>
-    <t>90 Elm St.</t>
-  </si>
-  <si>
-    <t>lee@example.edu</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>S20250006</t>
-  </si>
-  <si>
-    <t>Emily Brown</t>
-  </si>
-  <si>
-    <t>111 Oak Ave.</t>
-  </si>
-  <si>
-    <t>555-7890</t>
-  </si>
-  <si>
-    <t>brown@example.edu</t>
-  </si>
-  <si>
-    <t>Chem200</t>
-  </si>
-  <si>
-    <t>Synthesis and Characterization of Novel Catalysts</t>
-  </si>
-  <si>
-    <t>S20250007</t>
-  </si>
-  <si>
-    <t>George Smith</t>
-  </si>
-  <si>
-    <t>222 Pine Rd.</t>
-  </si>
-  <si>
-    <t>555-2345</t>
-  </si>
-  <si>
-    <t>smith@example.edu</t>
-  </si>
-  <si>
-    <t>Music102</t>
-  </si>
-  <si>
-    <t>S20250008</t>
-  </si>
-  <si>
-    <t>Helen Jones</t>
-  </si>
-  <si>
-    <t>333 Maple Dr.</t>
-  </si>
-  <si>
-    <t>555-4567</t>
-  </si>
-  <si>
-    <t>jones@example.edu</t>
-  </si>
-  <si>
-    <t>PSYCHO100, Music102, HIST101</t>
-  </si>
-  <si>
-    <t>The Effects of Stress on Cognitive Function</t>
-  </si>
-  <si>
-    <t>S20250009</t>
-  </si>
-  <si>
-    <t>Isaac Clark</t>
-  </si>
-  <si>
-    <t>444 Cedar Ln.</t>
-  </si>
-  <si>
-    <t>555-8901</t>
-  </si>
-  <si>
-    <t>clark@example.edu</t>
-  </si>
-  <si>
-    <t>BIo300</t>
-  </si>
-  <si>
-    <t>S20250010</t>
-  </si>
-  <si>
-    <t>555 Oakwood Pl.</t>
-  </si>
-  <si>
-    <t>davis@example.edu</t>
-  </si>
-  <si>
-    <t>The Renaissance: Art, Culture, and Society</t>
-  </si>
-  <si>
-    <t>Faculty ID</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Research Interest</t>
-  </si>
-  <si>
-    <t>Office Location</t>
-  </si>
-  <si>
-    <t>Courses Offered</t>
-  </si>
-  <si>
-    <t>F0001</t>
-  </si>
-  <si>
-    <t>Ph.D.</t>
-  </si>
-  <si>
-    <t>Computational Theory</t>
-  </si>
-  <si>
-    <t>turing@university.edu</t>
-  </si>
-  <si>
-    <t>F0002</t>
-  </si>
-  <si>
-    <t>Master's</t>
-  </si>
-  <si>
-    <t>English Literature</t>
-  </si>
-  <si>
-    <t>bronte@university.edu</t>
-  </si>
-  <si>
-    <t>F0003</t>
-  </si>
-  <si>
-    <t>Dr. Grace Hopper</t>
-  </si>
-  <si>
-    <t>Computer Programming</t>
-  </si>
-  <si>
-    <t>hopper@university.edu</t>
-  </si>
-  <si>
-    <t>Lab 203</t>
-  </si>
-  <si>
-    <t>Intro to Programming</t>
-  </si>
-  <si>
-    <t>F0004</t>
-  </si>
-  <si>
-    <t>copeland@university.edu</t>
-  </si>
-  <si>
-    <t>F0005</t>
-  </si>
-  <si>
-    <t>Albozr Gharabaghi</t>
-  </si>
-  <si>
-    <t>Water and Soil</t>
-  </si>
-  <si>
-    <t>gharabaghi@university.edu</t>
-  </si>
-  <si>
-    <t>Lab 202</t>
-  </si>
-  <si>
-    <t>Event Code</t>
-  </si>
-  <si>
-    <t>Event Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Date and Time</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Header Image</t>
-  </si>
-  <si>
-    <t>Registered Students</t>
-  </si>
-  <si>
-    <t>EV001</t>
-  </si>
-  <si>
-    <t>Welcome Seminar</t>
-  </si>
-  <si>
-    <t>Orientation week</t>
-  </si>
-  <si>
-    <t>Auditorium</t>
-  </si>
-  <si>
-    <t>Free</t>
-  </si>
-  <si>
-    <t>Alice Smith, Bob Johnson,Jennifer Davis,Helen Jones</t>
-  </si>
-  <si>
-    <t>EV002</t>
-  </si>
-  <si>
-    <t>Research Workshop</t>
-  </si>
-  <si>
-    <t>Graduate workshop</t>
-  </si>
-  <si>
-    <t>Lab 301</t>
-  </si>
-  <si>
-    <t>Paid ($20)</t>
-  </si>
-  <si>
-    <t>Alice Smith, Bob Johnson, Lucka Racki,Helen Jones,David Lee</t>
-  </si>
-  <si>
-    <t>ENG1210</t>
-  </si>
-  <si>
-    <t>Intro to Coding</t>
-  </si>
-  <si>
-    <t>undergraduate</t>
-  </si>
-  <si>
-    <t>qwe</t>
-  </si>
-  <si>
-    <t>Jennifer Russel</t>
-  </si>
-  <si>
-    <t>555-3457</t>
-  </si>
-  <si>
-    <t>40%</t>
-  </si>
-  <si>
-    <t>50%</t>
-  </si>
-  <si>
-    <t>60%</t>
-  </si>
-  <si>
-    <t>20%</t>
-  </si>
-  <si>
-    <t>default.png</t>
-  </si>
-  <si>
-    <t>2.png</t>
-  </si>
-  <si>
-    <t>OnePiece.jpg</t>
-  </si>
-  <si>
-    <t>default1234</t>
-  </si>
-  <si>
-    <t>F0006</t>
-  </si>
-  <si>
-    <t>penis</t>
-  </si>
-  <si>
-    <t>balls</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>doeakdasd</t>
+    <t>wer</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>dcv</t>
+  </si>
+  <si>
+    <t>334g</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>dfb</t>
+  </si>
+  <si>
+    <t>1345c</t>
+  </si>
+  <si>
+    <t>3e45</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>345c</t>
+  </si>
+  <si>
+    <t>gfd</t>
+  </si>
+  <si>
+    <t>qqqqq</t>
+  </si>
+  <si>
+    <t>wwwwwww</t>
+  </si>
+  <si>
+    <t>fff</t>
+  </si>
+  <si>
+    <t>eeeeee</t>
+  </si>
+  <si>
+    <t>ggg</t>
   </si>
 </sst>
 </file>
@@ -675,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -694,13 +709,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -922,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -959,42 +970,42 @@
     </row>
     <row r="4" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s" s="0">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s" s="0">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1004,1339 +1015,210 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E446E10-7AB3-43BE-BD1F-D9C9C032338B}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="16" width="12.33203125"/>
-    <col min="2" max="2" customWidth="true" style="6" width="27.0"/>
-    <col min="3" max="3" customWidth="true" style="6" width="12.6640625"/>
-    <col min="4" max="4" customWidth="true" style="6" width="15.44140625"/>
-    <col min="5" max="5" customWidth="true" style="16" width="8.6640625"/>
-    <col min="6" max="6" customWidth="true" style="6" width="16.88671875"/>
-    <col min="7" max="7" customWidth="true" style="20" width="20.5546875"/>
-    <col min="8" max="8" customWidth="true" style="6" width="9.5546875"/>
-    <col min="9" max="9" customWidth="true" style="6" width="16.5546875"/>
-    <col min="10" max="26" customWidth="true" style="6" width="10.88671875"/>
-    <col min="27" max="16384" style="6" width="12.5546875"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.41796875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.3046875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.44140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.21875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="13">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="14">
-        <v>30</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="16">
+        <v>46006.375</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="18">
-        <v>46006.375</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="13">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="16">
+        <v>46007.416666666664</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="13">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="14">
+      <c r="G4" s="16">
+        <v>46006.375</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="13">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="16">
+        <v>46007.416666666664</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="18">
-        <v>46007.416666666664</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="14">
-        <v>25</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="18">
-        <v>46007.416666666664</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>30</v>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>194</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>196</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>192</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="14">
-        <v>42</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="18">
-        <v>46007.520833333336</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="14">
-        <v>50</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="18">
-        <v>46005.166666666664</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="14">
-        <v>50</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="18">
-        <v>46005.166666666664</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="14">
-        <v>50</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="18">
-        <v>46005.166666666664</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="15">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="19">
-        <v>46004.416666666664</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
-        <v>5</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="15">
-        <v>25</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="19">
-        <v>46004.416666666664</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
-        <v>6</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="15">
-        <v>50</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="19">
-        <v>45992.375</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2344,7 +1226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D458A2-78A0-4890-A85A-AD55AFB8F75E}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -2360,420 +1242,420 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2797,171 +1679,171 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.0078125" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="16.8046875" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" width="7.65234375" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="20.1015625" bestFit="true"/>
-    <col min="5" max="5" customWidth="true" width="22.83203125" bestFit="true"/>
-    <col min="6" max="6" customWidth="true" width="12.91015625" bestFit="true"/>
-    <col min="7" max="7" customWidth="true" width="18.40625" bestFit="true"/>
-    <col min="8" max="8" customWidth="true" width="9.7109375" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.6640625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.77734375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.88671875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.44140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.6640625"/>
     <col min="9" max="26" customWidth="true" width="8.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3936,38 +2818,38 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001">
+    <row r="993" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1001" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1001" t="s" s="0">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="B1001" t="s" s="0">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C1001" t="s" s="0">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D1001" t="s" s="0">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="E1001" t="s" s="0">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="F1001" t="s" s="0">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G1001" t="s" s="0">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="H1001" t="s" s="0">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4001,96 +2883,96 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="18">
+        <v>150</v>
+      </c>
+      <c r="E2" s="16">
         <v>45901.416666666664</v>
       </c>
       <c r="F2" s="4">
         <v>100</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="18">
+        <v>156</v>
+      </c>
+      <c r="E3" s="16">
         <v>45935.583333333336</v>
       </c>
       <c r="F3" s="4">
         <v>50</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="20"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="20"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="21" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="22" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>